<commit_message>
completed all the Piece class with properties and methods. Made class abstract as all types of Piece will have their own movement and own getDestinations method. Also updated UML to show the small changes I made.
</commit_message>
<xml_diff>
--- a/ChessGameUML.xlsx
+++ b/ChessGameUML.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walid\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walid\Documents\Visual Studio 2017\Projects\ChessGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -205,6 +205,12 @@
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
             <a:t>- color : int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>-board : Board</a:t>
           </a:r>
         </a:p>
         <a:p>

</xml_diff>

<commit_message>
Created a BoardSpace struct. I also updated the Excel doc (UML)
</commit_message>
<xml_diff>
--- a/ChessGameUML.xlsx
+++ b/ChessGameUML.xlsx
@@ -77,16 +77,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>51436</xdr:rowOff>
+      <xdr:rowOff>89536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>74295</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>179070</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -101,7 +101,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="981075" y="2223136"/>
+          <a:off x="476250" y="2261236"/>
           <a:ext cx="2750820" cy="3120390"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -252,7 +252,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" i="1" baseline="0"/>
-            <a:t>+ getDestinations(int[] position)</a:t>
+            <a:t>+ getDestinations(int posX, int posY)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -270,16 +270,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -294,7 +294,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609599" y="190499"/>
+          <a:off x="1562099" y="200024"/>
           <a:ext cx="3648076" cy="1962151"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -345,7 +345,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- board : Piece[][]</a:t>
+            <a:t>- board : BoardSpace[][]</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -642,6 +642,133 @@
           <a:r>
             <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
             <a:t>+ promptDestinationSelect();</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>598170</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A780605-456C-409D-B927-2201B4BFA869}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3333750" y="2270761"/>
+          <a:ext cx="2750820" cy="1844039"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" b="1" i="0" u="none"/>
+            <a:t>BoardSpace</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100" b="1" i="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" u="none" baseline="0"/>
+            <a:t>------------------------------------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- occupied</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> : bool</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- isPossibleDestionation : bool</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- piece : Piece</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>------------------------------------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>+ getters and setters for all variables</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
+            <a:t>+ getBoardSpaceChar()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100" i="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
+            <a:t>Note : This class is a Struct</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -951,7 +1078,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Did some work on the Board class. Also update the UML accordingly.
</commit_message>
<xml_diff>
--- a/ChessGameUML.xlsx
+++ b/ChessGameUML.xlsx
@@ -351,13 +351,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- deadBlack : hashmap of Piece</a:t>
+            <a:t>- deadBlack : dictionary of Piece</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- deadWhite : hashmap of Piece</a:t>
+            <a:t>- deadWhite : dictionary of Piece</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -369,7 +369,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>+ getPiece(int x, int y)</a:t>
+            <a:t>+ getBoardSpace(int x, int y)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -382,12 +382,6 @@
           <a:r>
             <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
             <a:t>+ killPiece(int[] source)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
-            <a:t>+ isFinished()</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -528,6 +522,12 @@
           <a:r>
             <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
             <a:t>+ updatetextView()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
+            <a:t>+ isFinished()</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1078,7 +1078,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
created toString method for Board. Also updated UML
</commit_message>
<xml_diff>
--- a/ChessGameUML.xlsx
+++ b/ChessGameUML.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -385,6 +385,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
+            <a:t>+ toString()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
+            <a:t>     + dictionaryToString(dictionary of Piece)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-CA" sz="1100" i="0" baseline="0"/>
         </a:p>
       </xdr:txBody>
@@ -624,12 +636,6 @@
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
             <a:t>+ update()</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>+ update(jagged array of int[])</a:t>
           </a:r>
         </a:p>
         <a:p>

</xml_diff>

<commit_message>
Change Board so that dead Pieces are stored in LinkedList. It was the simplest solution to the duplicate key issue that would come up with Dictionary.
</commit_message>
<xml_diff>
--- a/ChessGameUML.xlsx
+++ b/ChessGameUML.xlsx
@@ -351,13 +351,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- deadBlack : dictionary of Piece</a:t>
+            <a:t>- deadBlack : LinkedList of Piece</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- deadWhite : dictionary of Piece</a:t>
+            <a:t>- deadWhite : LinkedList of Piece</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -393,7 +393,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" i="0" baseline="0"/>
-            <a:t>     + dictionaryToString(dictionary of Piece)</a:t>
+            <a:t>     + deadPiecesToString(dictionary of Piece)</a:t>
           </a:r>
         </a:p>
         <a:p>

</xml_diff>